<commit_message>
modif nicollini / ordinaire
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Documents/GitHub/mythographie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC66D9E2-10D6-3F4E-A810-34526A52090D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF0B770-9774-0F4A-AD34-B0E2F8DEF04A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{09C72171-0791-B248-913F-8D459B64DBA7}"/>
   </bookViews>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71520B63-331A-924F-BE2F-577EBBE4A982}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
ajout de nouveaux fichiers numérisés, (benucci, fontanella x2, lenoni) et maj fichier de suivi
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Documents/GitHub/mythographie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDBCCDB-B7DC-B241-97E3-ED0BDBA3A201}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528E476C-C9BF-9E40-8E61-9F2654A96E5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{09C72171-0791-B248-913F-8D459B64DBA7}"/>
+    <workbookView xWindow="6020" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{09C72171-0791-B248-913F-8D459B64DBA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>adams_myths-old-greece_1900.xml</t>
   </si>
@@ -139,6 +139,36 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>benucci_ristretto-analitico-01_1874.xml</t>
+  </si>
+  <si>
+    <t>durante_compendio-della-mitologia-01_1855.xml</t>
+  </si>
+  <si>
+    <t>fontanella_corso-di-mitologia-01_1806.xml</t>
+  </si>
+  <si>
+    <t>fontanella_corso-di-mitologia-02_1806.xml</t>
+  </si>
+  <si>
+    <t>leoni_interpretazione-de-miti_1855.xml</t>
+  </si>
+  <si>
+    <t>salomone_mitologia-iconologica_1841.xml</t>
+  </si>
+  <si>
+    <t>testi_mitologia-gioventu_1831.xml</t>
+  </si>
+  <si>
+    <t>tomeo_breve-corso_1824.xml</t>
+  </si>
+  <si>
+    <t>schèma à modifier pour validation</t>
+  </si>
+  <si>
+    <t>commentaires</t>
   </si>
 </sst>
 </file>
@@ -177,12 +207,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -212,7 +242,18 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -220,15 +261,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,19 +589,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71520B63-331A-924F-BE2F-577EBBE4A982}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -565,393 +612,525 @@
       <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="5">
-        <f>SUM(B2:B35)</f>
-        <v>34</v>
-      </c>
-      <c r="C36" s="5">
-        <f>SUM(C2:C35)</f>
-        <v>34</v>
-      </c>
+      <c r="B44" s="3">
+        <f>SUM(B2:B43)</f>
+        <v>41</v>
+      </c>
+      <c r="C44" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
maj suivi, pb intégration des images de testi mitologia gioventu
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Documents/GitHub/mythographie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528E476C-C9BF-9E40-8E61-9F2654A96E5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201B23DE-95D2-DF41-95B7-9195DEEA9999}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{09C72171-0791-B248-913F-8D459B64DBA7}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{09C72171-0791-B248-913F-8D459B64DBA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>adams_myths-old-greece_1900.xml</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>commentaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problème d'intégration des images dans le dépôt </t>
   </si>
 </sst>
 </file>
@@ -591,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71520B63-331A-924F-BE2F-577EBBE4A982}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1075,9 @@
       <c r="C39" s="2">
         <v>1</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">

</xml_diff>

<commit_message>
maj fichier de suivi
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Documents/GitHub/mythographie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201B23DE-95D2-DF41-95B7-9195DEEA9999}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E067815C-7CC2-2B42-8476-7B65CB816D9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{09C72171-0791-B248-913F-8D459B64DBA7}"/>
+    <workbookView xWindow="9720" yWindow="460" windowWidth="19080" windowHeight="16340" xr2:uid="{09C72171-0791-B248-913F-8D459B64DBA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>adams_myths-old-greece_1900.xml</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t xml:space="preserve">Problème d'intégration des images dans le dépôt </t>
+  </si>
+  <si>
+    <t>structure/encodage</t>
+  </si>
+  <si>
+    <t>images</t>
   </si>
 </sst>
 </file>
@@ -264,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -278,6 +284,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,20 +599,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71520B63-331A-924F-BE2F-577EBBE4A982}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -616,10 +625,16 @@
         <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -629,9 +644,15 @@
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -641,9 +662,15 @@
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -654,8 +681,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>38</v>
       </c>
@@ -666,8 +695,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -678,8 +709,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -690,8 +723,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -702,8 +737,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -714,8 +751,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -726,8 +765,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -738,8 +779,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -750,8 +793,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
@@ -762,8 +807,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -774,8 +821,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -786,8 +835,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -798,8 +849,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -810,8 +863,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
@@ -822,8 +877,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>41</v>
       </c>
@@ -833,11 +890,13 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
@@ -848,8 +907,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
@@ -860,8 +921,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -872,8 +935,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
@@ -884,8 +949,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
@@ -896,8 +963,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
@@ -908,8 +977,10 @@
         <v>1</v>
       </c>
       <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -920,8 +991,10 @@
         <v>1</v>
       </c>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
@@ -932,8 +1005,10 @@
         <v>1</v>
       </c>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
@@ -944,8 +1019,10 @@
         <v>1</v>
       </c>
       <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
@@ -956,8 +1033,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
@@ -968,8 +1047,10 @@
         <v>1</v>
       </c>
       <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>24</v>
       </c>
@@ -980,8 +1061,10 @@
         <v>1</v>
       </c>
       <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>25</v>
       </c>
@@ -992,8 +1075,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
@@ -1004,8 +1089,10 @@
         <v>1</v>
       </c>
       <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>27</v>
       </c>
@@ -1016,8 +1103,10 @@
         <v>1</v>
       </c>
       <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
@@ -1028,8 +1117,10 @@
         <v>1</v>
       </c>
       <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>29</v>
       </c>
@@ -1040,8 +1131,10 @@
         <v>1</v>
       </c>
       <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
@@ -1052,8 +1145,10 @@
         <v>1</v>
       </c>
       <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>30</v>
       </c>
@@ -1064,8 +1159,10 @@
         <v>1</v>
       </c>
       <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>44</v>
       </c>
@@ -1075,11 +1172,13 @@
       <c r="C39" s="2">
         <v>1</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>45</v>
       </c>
@@ -1090,8 +1189,10 @@
         <v>1</v>
       </c>
       <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>31</v>
       </c>
@@ -1102,8 +1203,10 @@
         <v>1</v>
       </c>
       <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>32</v>
       </c>
@@ -1114,8 +1217,10 @@
         <v>1</v>
       </c>
       <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>33</v>
       </c>
@@ -1125,9 +1230,11 @@
       <c r="C43" s="7">
         <v>1</v>
       </c>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>37</v>
       </c>
@@ -1136,6 +1243,8 @@
         <v>41</v>
       </c>
       <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>